<commit_message>
nmv 01 12 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.2 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.2 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AA3738-9CDA-486E-A6BE-2254A28A36FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA32A061-2E97-4A71-9794-853BCEDAA0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6303,7 +6303,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6439,8 +6439,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6468,6 +6473,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6499,7 +6510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -6664,6 +6675,9 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6948,9 +6962,9 @@
   <dimension ref="A1:V2500"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1409" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1424" sqref="N1424"/>
+      <selection pane="bottomLeft" activeCell="N142" sqref="N142:N639"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -12836,7 +12850,7 @@
         <f t="shared" si="8"/>
         <v>141</v>
       </c>
-      <c r="N142" s="37" t="s">
+      <c r="N142" s="57" t="s">
         <v>261</v>
       </c>
       <c r="O142" s="6" t="s">
@@ -30322,7 +30336,7 @@
         <f t="shared" si="29"/>
         <v>168</v>
       </c>
-      <c r="N639" s="37" t="s">
+      <c r="N639" s="57" t="s">
         <v>261</v>
       </c>
       <c r="O639" s="6" t="s">

</xml_diff>

<commit_message>
nmv 03 12 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.2 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.2 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3461247A-1CDE-408C-B016-6F8511411DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13C55D4-2103-4EB2-A031-E3502E222210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7130" uniqueCount="2087">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7131" uniqueCount="2089">
   <si>
     <t>PS</t>
   </si>
@@ -6239,9 +6239,6 @@
     <t>Table Process</t>
   </si>
   <si>
-    <t>sauShadhIShu</t>
-  </si>
-  <si>
     <t>P[r]</t>
   </si>
   <si>
@@ -6297,13 +6294,22 @@
   </si>
   <si>
     <t>viqSvaPsni#yA</t>
+  </si>
+  <si>
+    <t>sauShadI</t>
+  </si>
+  <si>
+    <t>yo &amp;nu, yo &amp;nvanu</t>
+  </si>
+  <si>
+    <t>yo &amp;nu + yo anvanu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6449,8 +6455,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6465,12 +6477,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -6478,6 +6484,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6509,7 +6533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -6654,12 +6678,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -6669,39 +6687,63 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6983,12 +7025,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V2500"/>
+  <dimension ref="A1:X2500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A925" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2486" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="I936" sqref="I936:V936"/>
+      <selection pane="bottomLeft" activeCell="Q2452" sqref="Q2452"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -7012,7 +7054,9 @@
     <col min="20" max="20" width="23.140625" style="1" customWidth="1"/>
     <col min="21" max="21" width="18.5703125" style="1" customWidth="1"/>
     <col min="22" max="22" width="62.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="263" width="9.140625" style="2"/>
+    <col min="23" max="23" width="9.140625" style="2"/>
+    <col min="24" max="24" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="263" width="9.140625" style="2"/>
     <col min="264" max="264" width="9.28515625" style="2" customWidth="1"/>
     <col min="265" max="266" width="9.140625" style="2"/>
     <col min="267" max="267" width="54.42578125" style="2" customWidth="1"/>
@@ -7930,7 +7974,7 @@
       <c r="N11" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="O11" s="56" t="s">
+      <c r="O11" s="54" t="s">
         <v>1</v>
       </c>
       <c r="P11" s="11"/>
@@ -8571,7 +8615,7 @@
       <c r="N27" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="O27" s="56" t="s">
+      <c r="O27" s="54" t="s">
         <v>1</v>
       </c>
       <c r="P27" s="11"/>
@@ -9243,7 +9287,7 @@
       <c r="N44" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="O44" s="56" t="s">
+      <c r="O44" s="54" t="s">
         <v>1</v>
       </c>
       <c r="P44" s="11"/>
@@ -9906,7 +9950,7 @@
       <c r="N61" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="O61" s="56" t="s">
+      <c r="O61" s="54" t="s">
         <v>1</v>
       </c>
       <c r="P61" s="11"/>
@@ -11032,7 +11076,7 @@
         <f t="shared" si="5"/>
         <v>90</v>
       </c>
-      <c r="N91" s="37" t="s">
+      <c r="N91" s="66" t="s">
         <v>232</v>
       </c>
       <c r="O91" s="6" t="s">
@@ -11077,7 +11121,7 @@
         <f t="shared" si="5"/>
         <v>91</v>
       </c>
-      <c r="N92" s="37" t="s">
+      <c r="N92" s="66" t="s">
         <v>233</v>
       </c>
       <c r="O92" s="6"/>
@@ -12202,7 +12246,7 @@
         <v>90</v>
       </c>
       <c r="T123" s="6" t="s">
-        <v>183</v>
+        <v>2060</v>
       </c>
       <c r="U123" s="6"/>
       <c r="V123" s="37"/>
@@ -12874,8 +12918,8 @@
         <f t="shared" si="8"/>
         <v>141</v>
       </c>
-      <c r="N142" s="57" t="s">
-        <v>2086</v>
+      <c r="N142" s="55" t="s">
+        <v>2085</v>
       </c>
       <c r="O142" s="6" t="s">
         <v>0</v>
@@ -12951,7 +12995,7 @@
       <c r="N144" s="37" t="s">
         <v>349</v>
       </c>
-      <c r="O144" s="56" t="s">
+      <c r="O144" s="54" t="s">
         <v>1</v>
       </c>
       <c r="P144" s="11" t="s">
@@ -13732,7 +13776,7 @@
         <f t="shared" si="8"/>
         <v>165</v>
       </c>
-      <c r="N166" s="37" t="s">
+      <c r="N166" s="65" t="s">
         <v>279</v>
       </c>
       <c r="O166" s="5"/>
@@ -13772,7 +13816,7 @@
         <f t="shared" si="8"/>
         <v>166</v>
       </c>
-      <c r="N167" s="37" t="s">
+      <c r="N167" s="65" t="s">
         <v>280</v>
       </c>
       <c r="O167" s="6"/>
@@ -14194,7 +14238,7 @@
         <f t="shared" si="8"/>
         <v>178</v>
       </c>
-      <c r="N179" s="37" t="s">
+      <c r="N179" s="65" t="s">
         <v>230</v>
       </c>
       <c r="O179" s="5"/>
@@ -14951,7 +14995,7 @@
         <f t="shared" si="11"/>
         <v>200</v>
       </c>
-      <c r="N201" s="37" t="s">
+      <c r="N201" s="65" t="s">
         <v>304</v>
       </c>
       <c r="O201" s="5"/>
@@ -14986,7 +15030,7 @@
         <f t="shared" si="11"/>
         <v>201</v>
       </c>
-      <c r="N202" s="37" t="s">
+      <c r="N202" s="65" t="s">
         <v>305</v>
       </c>
       <c r="O202" s="6" t="s">
@@ -15058,7 +15102,7 @@
         <f t="shared" si="11"/>
         <v>203</v>
       </c>
-      <c r="N204" s="37" t="s">
+      <c r="N204" s="65" t="s">
         <v>255</v>
       </c>
       <c r="O204" s="5"/>
@@ -15337,7 +15381,7 @@
         <f t="shared" si="11"/>
         <v>211</v>
       </c>
-      <c r="N212" s="37" t="s">
+      <c r="N212" s="65" t="s">
         <v>232</v>
       </c>
       <c r="O212" s="5" t="s">
@@ -15374,7 +15418,7 @@
         <f t="shared" si="11"/>
         <v>212</v>
       </c>
-      <c r="N213" s="37" t="s">
+      <c r="N213" s="65" t="s">
         <v>312</v>
       </c>
       <c r="O213" s="5"/>
@@ -15623,7 +15667,7 @@
         <f t="shared" si="11"/>
         <v>219</v>
       </c>
-      <c r="N220" s="37" t="s">
+      <c r="N220" s="65" t="s">
         <v>255</v>
       </c>
       <c r="O220" s="6"/>
@@ -16165,7 +16209,7 @@
         <f t="shared" si="11"/>
         <v>235</v>
       </c>
-      <c r="N236" s="37" t="s">
+      <c r="N236" s="65" t="s">
         <v>255</v>
       </c>
       <c r="O236" s="5"/>
@@ -16612,7 +16656,7 @@
         <f t="shared" si="11"/>
         <v>248</v>
       </c>
-      <c r="N249" s="37" t="s">
+      <c r="N249" s="65" t="s">
         <v>1645</v>
       </c>
       <c r="O249" s="6"/>
@@ -17442,7 +17486,7 @@
     </row>
     <row r="271" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A271" s="6"/>
-      <c r="D271" s="52" t="s">
+      <c r="D271" s="50" t="s">
         <v>2063</v>
       </c>
       <c r="I271" s="39" t="s">
@@ -17477,7 +17521,7 @@
     </row>
     <row r="272" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A272" s="6"/>
-      <c r="D272" s="52" t="s">
+      <c r="D272" s="50" t="s">
         <v>2063</v>
       </c>
       <c r="I272" s="39" t="s">
@@ -17997,7 +18041,7 @@
         <f t="shared" si="14"/>
         <v>19</v>
       </c>
-      <c r="N286" s="37" t="s">
+      <c r="N286" s="53" t="s">
         <v>242</v>
       </c>
       <c r="O286" s="5"/>
@@ -18031,7 +18075,7 @@
         <f t="shared" si="14"/>
         <v>20</v>
       </c>
-      <c r="N287" s="37" t="s">
+      <c r="N287" s="53" t="s">
         <v>255</v>
       </c>
       <c r="O287" s="5"/>
@@ -18987,7 +19031,7 @@
         <f t="shared" si="14"/>
         <v>47</v>
       </c>
-      <c r="N314" s="37" t="s">
+      <c r="N314" s="53" t="s">
         <v>255</v>
       </c>
       <c r="O314" s="5"/>
@@ -20240,7 +20284,7 @@
         <f t="shared" si="17"/>
         <v>83</v>
       </c>
-      <c r="N350" s="37" t="s">
+      <c r="N350" s="53" t="s">
         <v>214</v>
       </c>
       <c r="O350" s="5"/>
@@ -20275,7 +20319,7 @@
         <f t="shared" si="17"/>
         <v>84</v>
       </c>
-      <c r="N351" s="37" t="s">
+      <c r="N351" s="53" t="s">
         <v>386</v>
       </c>
       <c r="O351" s="6"/>
@@ -20885,7 +20929,7 @@
     </row>
     <row r="369" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A369" s="6"/>
-      <c r="D369" s="52" t="s">
+      <c r="D369" s="50" t="s">
         <v>2064</v>
       </c>
       <c r="H369" s="44" t="s">
@@ -20923,7 +20967,7 @@
     </row>
     <row r="370" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A370" s="6"/>
-      <c r="D370" s="52" t="s">
+      <c r="D370" s="50" t="s">
         <v>2064</v>
       </c>
       <c r="H370" s="44" t="s">
@@ -21664,7 +21708,7 @@
         <f t="shared" si="20"/>
         <v>124</v>
       </c>
-      <c r="N391" s="37" t="s">
+      <c r="N391" s="53" t="s">
         <v>354</v>
       </c>
       <c r="O391" s="6" t="s">
@@ -21703,7 +21747,7 @@
         <f t="shared" si="20"/>
         <v>125</v>
       </c>
-      <c r="N392" s="37" t="s">
+      <c r="N392" s="53" t="s">
         <v>416</v>
       </c>
       <c r="O392" s="5"/>
@@ -21804,7 +21848,7 @@
         <f t="shared" si="20"/>
         <v>128</v>
       </c>
-      <c r="N395" s="37" t="s">
+      <c r="N395" s="53" t="s">
         <v>417</v>
       </c>
       <c r="O395" s="6"/>
@@ -21923,7 +21967,7 @@
     </row>
     <row r="399" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A399" s="6"/>
-      <c r="D399" s="52" t="s">
+      <c r="D399" s="50" t="s">
         <v>2065</v>
       </c>
       <c r="I399" s="39" t="s">
@@ -21958,7 +22002,7 @@
     </row>
     <row r="400" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A400" s="6"/>
-      <c r="D400" s="52" t="s">
+      <c r="D400" s="50" t="s">
         <v>2065</v>
       </c>
       <c r="I400" s="39" t="s">
@@ -22131,7 +22175,7 @@
     </row>
     <row r="405" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A405" s="6"/>
-      <c r="D405" s="53"/>
+      <c r="D405" s="51"/>
       <c r="I405" s="39" t="s">
         <v>31</v>
       </c>
@@ -22187,7 +22231,7 @@
         <f t="shared" si="20"/>
         <v>139</v>
       </c>
-      <c r="N406" s="37" t="s">
+      <c r="N406" s="53" t="s">
         <v>255</v>
       </c>
       <c r="O406" s="5"/>
@@ -22728,7 +22772,7 @@
         <f t="shared" si="20"/>
         <v>154</v>
       </c>
-      <c r="N421" s="37" t="s">
+      <c r="N421" s="53" t="s">
         <v>255</v>
       </c>
       <c r="O421" s="5"/>
@@ -22766,7 +22810,7 @@
         <f t="shared" si="20"/>
         <v>155</v>
       </c>
-      <c r="N422" s="37" t="s">
+      <c r="N422" s="53" t="s">
         <v>434</v>
       </c>
       <c r="O422" s="6" t="s">
@@ -23088,7 +23132,7 @@
       <c r="N431" s="37" t="s">
         <v>262</v>
       </c>
-      <c r="O431" s="56" t="s">
+      <c r="O431" s="54" t="s">
         <v>1</v>
       </c>
       <c r="P431" s="6"/>
@@ -23198,7 +23242,7 @@
       <c r="N434" s="37" t="s">
         <v>262</v>
       </c>
-      <c r="O434" s="56" t="s">
+      <c r="O434" s="54" t="s">
         <v>1</v>
       </c>
       <c r="P434" s="6"/>
@@ -23305,7 +23349,7 @@
         <f t="shared" si="20"/>
         <v>170</v>
       </c>
-      <c r="N437" s="37" t="s">
+      <c r="N437" s="53" t="s">
         <v>255</v>
       </c>
       <c r="O437" s="6"/>
@@ -24194,7 +24238,7 @@
         <f t="shared" si="23"/>
         <v>196</v>
       </c>
-      <c r="N463" s="37" t="s">
+      <c r="N463" s="53" t="s">
         <v>214</v>
       </c>
       <c r="O463" s="5"/>
@@ -24229,7 +24273,7 @@
         <f t="shared" si="23"/>
         <v>197</v>
       </c>
-      <c r="N464" s="37" t="s">
+      <c r="N464" s="53" t="s">
         <v>386</v>
       </c>
       <c r="O464" s="5"/>
@@ -24555,7 +24599,7 @@
         <f t="shared" si="23"/>
         <v>2</v>
       </c>
-      <c r="N473" s="37" t="s">
+      <c r="N473" s="66" t="s">
         <v>464</v>
       </c>
       <c r="O473" s="6"/>
@@ -24593,7 +24637,7 @@
         <f t="shared" si="23"/>
         <v>3</v>
       </c>
-      <c r="N474" s="37" t="s">
+      <c r="N474" s="66" t="s">
         <v>233</v>
       </c>
       <c r="O474" s="5"/>
@@ -25021,10 +25065,10 @@
         <f t="shared" si="23"/>
         <v>15</v>
       </c>
-      <c r="N486" s="37" t="s">
+      <c r="N486" s="53" t="s">
         <v>262</v>
       </c>
-      <c r="O486" s="58" t="s">
+      <c r="O486" s="56" t="s">
         <v>1</v>
       </c>
       <c r="P486" s="6"/>
@@ -25059,7 +25103,7 @@
         <f t="shared" si="23"/>
         <v>16</v>
       </c>
-      <c r="N487" s="37" t="s">
+      <c r="N487" s="53" t="s">
         <v>472</v>
       </c>
       <c r="O487" s="5"/>
@@ -25099,7 +25143,7 @@
         <f t="shared" si="23"/>
         <v>17</v>
       </c>
-      <c r="N488" s="37" t="s">
+      <c r="N488" s="53" t="s">
         <v>277</v>
       </c>
       <c r="O488" s="6"/>
@@ -26797,7 +26841,7 @@
         <f t="shared" si="26"/>
         <v>66</v>
       </c>
-      <c r="N537" s="37" t="s">
+      <c r="N537" s="53" t="s">
         <v>232</v>
       </c>
       <c r="O537" s="5" t="s">
@@ -26834,7 +26878,7 @@
         <f t="shared" si="26"/>
         <v>67</v>
       </c>
-      <c r="N538" s="37" t="s">
+      <c r="N538" s="53" t="s">
         <v>418</v>
       </c>
       <c r="O538" s="5"/>
@@ -27032,7 +27076,7 @@
         <f t="shared" si="26"/>
         <v>73</v>
       </c>
-      <c r="N544" s="37" t="s">
+      <c r="N544" s="53" t="s">
         <v>338</v>
       </c>
       <c r="O544" s="5"/>
@@ -27067,7 +27111,7 @@
         <f t="shared" si="26"/>
         <v>74</v>
       </c>
-      <c r="N545" s="37" t="s">
+      <c r="N545" s="53" t="s">
         <v>322</v>
       </c>
       <c r="O545" s="5"/>
@@ -27899,7 +27943,7 @@
         <f t="shared" si="26"/>
         <v>98</v>
       </c>
-      <c r="N569" s="37" t="s">
+      <c r="N569" s="53" t="s">
         <v>255</v>
       </c>
       <c r="O569" s="5"/>
@@ -27937,7 +27981,7 @@
         <f t="shared" si="26"/>
         <v>99</v>
       </c>
-      <c r="N570" s="37" t="s">
+      <c r="N570" s="65" t="s">
         <v>525</v>
       </c>
       <c r="O570" s="5"/>
@@ -27977,7 +28021,7 @@
         <f t="shared" si="26"/>
         <v>100</v>
       </c>
-      <c r="N571" s="37" t="s">
+      <c r="N571" s="65" t="s">
         <v>274</v>
       </c>
       <c r="O571" s="5"/>
@@ -27990,10 +28034,9 @@
       <c r="V571" s="37"/>
     </row>
     <row r="572" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A572" s="50" t="s">
-        <v>2067</v>
-      </c>
-      <c r="B572" s="51"/>
+      <c r="A572" s="64" t="s">
+        <v>2086</v>
+      </c>
       <c r="D572" s="19"/>
       <c r="I572" s="39" t="s">
         <v>35</v>
@@ -28012,7 +28055,7 @@
         <f t="shared" si="26"/>
         <v>101</v>
       </c>
-      <c r="N572" s="37" t="s">
+      <c r="N572" s="63" t="s">
         <v>199</v>
       </c>
       <c r="O572" s="5"/>
@@ -28045,7 +28088,7 @@
         <f t="shared" si="26"/>
         <v>102</v>
       </c>
-      <c r="N573" s="37" t="s">
+      <c r="N573" s="67" t="s">
         <v>526</v>
       </c>
       <c r="O573" s="6"/>
@@ -28078,7 +28121,7 @@
         <f t="shared" si="26"/>
         <v>103</v>
       </c>
-      <c r="N574" s="37" t="s">
+      <c r="N574" s="67" t="s">
         <v>195</v>
       </c>
       <c r="O574" s="5" t="s">
@@ -28264,7 +28307,7 @@
         <v>90</v>
       </c>
       <c r="T579" s="6" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="U579" s="6"/>
       <c r="V579" s="37" t="s">
@@ -28818,7 +28861,7 @@
         <f t="shared" si="29"/>
         <v>124</v>
       </c>
-      <c r="N595" s="37" t="s">
+      <c r="N595" s="53" t="s">
         <v>535</v>
       </c>
       <c r="O595" s="6"/>
@@ -28919,7 +28962,7 @@
         <f t="shared" si="29"/>
         <v>127</v>
       </c>
-      <c r="N598" s="37" t="s">
+      <c r="N598" s="53" t="s">
         <v>255</v>
       </c>
       <c r="O598" s="5"/>
@@ -29316,7 +29359,7 @@
         <f t="shared" si="29"/>
         <v>138</v>
       </c>
-      <c r="N609" s="37" t="s">
+      <c r="N609" s="53" t="s">
         <v>535</v>
       </c>
       <c r="O609" s="5"/>
@@ -29419,7 +29462,7 @@
         <f t="shared" si="29"/>
         <v>141</v>
       </c>
-      <c r="N612" s="37" t="s">
+      <c r="N612" s="53" t="s">
         <v>255</v>
       </c>
       <c r="O612" s="5"/>
@@ -29633,7 +29676,7 @@
         <f t="shared" si="29"/>
         <v>147</v>
       </c>
-      <c r="N618" s="37" t="s">
+      <c r="N618" s="53" t="s">
         <v>543</v>
       </c>
       <c r="O618" s="5"/>
@@ -29668,7 +29711,7 @@
         <f t="shared" si="29"/>
         <v>148</v>
       </c>
-      <c r="N619" s="37" t="s">
+      <c r="N619" s="53" t="s">
         <v>477</v>
       </c>
       <c r="O619" s="6" t="s">
@@ -29881,7 +29924,7 @@
         <f t="shared" si="29"/>
         <v>154</v>
       </c>
-      <c r="N625" s="37" t="s">
+      <c r="N625" s="66" t="s">
         <v>255</v>
       </c>
       <c r="O625" s="5"/>
@@ -30263,7 +30306,7 @@
         <f t="shared" si="29"/>
         <v>165</v>
       </c>
-      <c r="N636" s="37" t="s">
+      <c r="N636" s="53" t="s">
         <v>230</v>
       </c>
       <c r="O636" s="5"/>
@@ -30366,8 +30409,8 @@
         <f t="shared" si="29"/>
         <v>168</v>
       </c>
-      <c r="N639" s="57" t="s">
-        <v>2086</v>
+      <c r="N639" s="55" t="s">
+        <v>2085</v>
       </c>
       <c r="O639" s="6" t="s">
         <v>0</v>
@@ -30443,7 +30486,7 @@
       <c r="N641" s="37" t="s">
         <v>349</v>
       </c>
-      <c r="O641" s="58" t="s">
+      <c r="O641" s="56" t="s">
         <v>1</v>
       </c>
       <c r="P641" s="11" t="s">
@@ -31198,7 +31241,7 @@
         <f t="shared" si="32"/>
         <v>192</v>
       </c>
-      <c r="N663" s="37" t="s">
+      <c r="N663" s="53" t="s">
         <v>557</v>
       </c>
       <c r="O663" s="5"/>
@@ -31233,7 +31276,7 @@
         <f t="shared" si="32"/>
         <v>193</v>
       </c>
-      <c r="N664" s="37" t="s">
+      <c r="N664" s="53" t="s">
         <v>558</v>
       </c>
       <c r="O664" s="6"/>
@@ -31475,7 +31518,7 @@
         <f t="shared" si="32"/>
         <v>200</v>
       </c>
-      <c r="N671" s="37" t="s">
+      <c r="N671" s="53" t="s">
         <v>564</v>
       </c>
       <c r="O671" s="5" t="s">
@@ -31513,7 +31556,7 @@
         <f t="shared" si="32"/>
         <v>201</v>
       </c>
-      <c r="N672" s="37" t="s">
+      <c r="N672" s="53" t="s">
         <v>563</v>
       </c>
       <c r="O672" s="5"/>
@@ -31702,7 +31745,7 @@
         <f t="shared" si="32"/>
         <v>207</v>
       </c>
-      <c r="N678" s="37" t="s">
+      <c r="N678" s="53" t="s">
         <v>255</v>
       </c>
       <c r="O678" s="6"/>
@@ -32113,7 +32156,7 @@
       <c r="N690" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="O690" s="58" t="s">
+      <c r="O690" s="56" t="s">
         <v>1</v>
       </c>
       <c r="P690" s="6"/>
@@ -32183,7 +32226,7 @@
       <c r="N692" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="O692" s="58" t="s">
+      <c r="O692" s="56" t="s">
         <v>1</v>
       </c>
       <c r="P692" s="6"/>
@@ -32284,7 +32327,7 @@
         <f t="shared" si="32"/>
         <v>8</v>
       </c>
-      <c r="N695" s="37" t="s">
+      <c r="N695" s="53" t="s">
         <v>577</v>
       </c>
       <c r="O695" s="5"/>
@@ -32320,7 +32363,7 @@
         <f t="shared" si="32"/>
         <v>9</v>
       </c>
-      <c r="N696" s="37" t="s">
+      <c r="N696" s="53" t="s">
         <v>578</v>
       </c>
       <c r="O696" s="5"/>
@@ -33652,7 +33695,7 @@
         <f t="shared" si="35"/>
         <v>50</v>
       </c>
-      <c r="N737" s="37" t="s">
+      <c r="N737" s="53" t="s">
         <v>602</v>
       </c>
       <c r="O737" s="5"/>
@@ -33684,7 +33727,7 @@
         <f t="shared" si="35"/>
         <v>51</v>
       </c>
-      <c r="N738" s="37" t="s">
+      <c r="N738" s="53" t="s">
         <v>603</v>
       </c>
       <c r="O738" s="6" t="s">
@@ -35680,7 +35723,7 @@
         <f t="shared" si="38"/>
         <v>111</v>
       </c>
-      <c r="N798" s="37" t="s">
+      <c r="N798" s="68" t="s">
         <v>637</v>
       </c>
       <c r="O798" s="5"/>
@@ -35783,7 +35826,7 @@
         <f t="shared" si="38"/>
         <v>114</v>
       </c>
-      <c r="N801" s="37" t="s">
+      <c r="N801" s="68" t="s">
         <v>639</v>
       </c>
       <c r="O801" s="5"/>
@@ -36129,7 +36172,7 @@
         <f t="shared" si="38"/>
         <v>124</v>
       </c>
-      <c r="N811" s="37" t="s">
+      <c r="N811" s="68" t="s">
         <v>255</v>
       </c>
       <c r="O811" s="5"/>
@@ -36590,7 +36633,7 @@
         <f t="shared" si="38"/>
         <v>138</v>
       </c>
-      <c r="N825" s="37" t="s">
+      <c r="N825" s="68" t="s">
         <v>242</v>
       </c>
       <c r="O825" s="5"/>
@@ -36624,7 +36667,7 @@
         <f t="shared" si="38"/>
         <v>139</v>
       </c>
-      <c r="N826" s="37" t="s">
+      <c r="N826" s="68" t="s">
         <v>656</v>
       </c>
       <c r="O826" s="6" t="s">
@@ -37027,7 +37070,7 @@
         <f t="shared" si="41"/>
         <v>151</v>
       </c>
-      <c r="N838" s="37" t="s">
+      <c r="N838" s="68" t="s">
         <v>255</v>
       </c>
       <c r="O838" s="5"/>
@@ -37124,7 +37167,7 @@
         <f t="shared" si="41"/>
         <v>154</v>
       </c>
-      <c r="N841" s="37" t="s">
+      <c r="N841" s="68" t="s">
         <v>270</v>
       </c>
       <c r="O841" s="5"/>
@@ -37159,7 +37202,7 @@
         <f t="shared" si="41"/>
         <v>155</v>
       </c>
-      <c r="N842" s="37" t="s">
+      <c r="N842" s="68" t="s">
         <v>233</v>
       </c>
       <c r="O842" s="6"/>
@@ -38185,7 +38228,7 @@
         <f t="shared" si="41"/>
         <v>187</v>
       </c>
-      <c r="N874" s="37" t="s">
+      <c r="N874" s="68" t="s">
         <v>674</v>
       </c>
       <c r="O874" s="5"/>
@@ -38222,7 +38265,7 @@
         <f t="shared" si="41"/>
         <v>188</v>
       </c>
-      <c r="N875" s="37" t="s">
+      <c r="N875" s="68" t="s">
         <v>675</v>
       </c>
       <c r="O875" s="6" t="s">
@@ -38320,7 +38363,7 @@
         <v>191</v>
       </c>
       <c r="N878" s="37" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="O878" s="5"/>
       <c r="P878" s="11" t="s">
@@ -38332,7 +38375,7 @@
       <c r="T878" s="6"/>
       <c r="U878" s="6"/>
       <c r="V878" s="37" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="879" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38525,7 +38568,7 @@
     </row>
     <row r="885" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A885" s="6" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
       <c r="I885" s="39" t="s">
         <v>40</v>
@@ -39239,8 +39282,8 @@
       <c r="V905" s="37"/>
     </row>
     <row r="906" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="D906" s="54" t="s">
-        <v>2072</v>
+      <c r="D906" s="52" t="s">
+        <v>2071</v>
       </c>
       <c r="H906" s="30"/>
       <c r="I906" s="39" t="s">
@@ -39691,7 +39734,7 @@
         <f t="shared" si="44"/>
         <v>34</v>
       </c>
-      <c r="N919" s="37" t="s">
+      <c r="N919" s="68" t="s">
         <v>255</v>
       </c>
       <c r="O919" s="5"/>
@@ -40083,7 +40126,7 @@
         <f t="shared" si="44"/>
         <v>46</v>
       </c>
-      <c r="N931" s="37" t="s">
+      <c r="N931" s="68" t="s">
         <v>1645</v>
       </c>
       <c r="O931" s="5"/>
@@ -40234,36 +40277,36 @@
       </c>
     </row>
     <row r="936" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I936" s="61" t="s">
+      <c r="I936" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="J936" s="62">
+      <c r="J936" s="59">
         <v>19</v>
       </c>
-      <c r="K936" s="61">
+      <c r="K936" s="58">
         <f t="shared" si="42"/>
         <v>935</v>
       </c>
-      <c r="L936" s="61">
+      <c r="L936" s="58">
         <v>1</v>
       </c>
-      <c r="M936" s="61">
+      <c r="M936" s="58">
         <f t="shared" si="44"/>
         <v>51</v>
       </c>
-      <c r="N936" s="63" t="s">
+      <c r="N936" s="60" t="s">
         <v>1693</v>
       </c>
-      <c r="O936" s="64"/>
-      <c r="P936" s="65" t="s">
+      <c r="O936" s="61"/>
+      <c r="P936" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="Q936" s="66"/>
-      <c r="R936" s="66"/>
-      <c r="S936" s="66"/>
-      <c r="T936" s="66"/>
-      <c r="U936" s="66"/>
-      <c r="V936" s="63" t="s">
+      <c r="Q936" s="12"/>
+      <c r="R936" s="12"/>
+      <c r="S936" s="12"/>
+      <c r="T936" s="12"/>
+      <c r="U936" s="12"/>
+      <c r="V936" s="60" t="s">
         <v>1902</v>
       </c>
     </row>
@@ -40558,9 +40601,7 @@
       <c r="P945" s="6"/>
       <c r="Q945" s="6"/>
       <c r="R945" s="6"/>
-      <c r="S945" s="6" t="s">
-        <v>184</v>
-      </c>
+      <c r="S945" s="6"/>
       <c r="T945" s="6"/>
       <c r="U945" s="6"/>
       <c r="V945" s="37"/>
@@ -40777,7 +40818,7 @@
         <f t="shared" si="44"/>
         <v>67</v>
       </c>
-      <c r="N952" s="37" t="s">
+      <c r="N952" s="68" t="s">
         <v>405</v>
       </c>
       <c r="O952" s="5"/>
@@ -40813,7 +40854,7 @@
         <f t="shared" si="44"/>
         <v>68</v>
       </c>
-      <c r="N953" s="37" t="s">
+      <c r="N953" s="68" t="s">
         <v>707</v>
       </c>
       <c r="O953" s="5"/>
@@ -41289,7 +41330,7 @@
         <f t="shared" si="47"/>
         <v>82</v>
       </c>
-      <c r="N967" s="37" t="s">
+      <c r="N967" s="68" t="s">
         <v>557</v>
       </c>
       <c r="O967" s="5"/>
@@ -41322,7 +41363,7 @@
         <f t="shared" si="47"/>
         <v>83</v>
       </c>
-      <c r="N968" s="37" t="s">
+      <c r="N968" s="68" t="s">
         <v>716</v>
       </c>
       <c r="O968" s="5"/>
@@ -42896,7 +42937,7 @@
         <f t="shared" si="47"/>
         <v>131</v>
       </c>
-      <c r="N1016" s="37" t="s">
+      <c r="N1016" s="68" t="s">
         <v>270</v>
       </c>
       <c r="O1016" s="5"/>
@@ -42931,7 +42972,7 @@
         <f t="shared" si="47"/>
         <v>132</v>
       </c>
-      <c r="N1017" s="37" t="s">
+      <c r="N1017" s="68" t="s">
         <v>744</v>
       </c>
       <c r="O1017" s="6"/>
@@ -42993,7 +43034,7 @@
         <f t="shared" si="47"/>
         <v>134</v>
       </c>
-      <c r="N1019" s="37" t="s">
+      <c r="N1019" s="68" t="s">
         <v>746</v>
       </c>
       <c r="O1019" s="5"/>
@@ -43026,7 +43067,7 @@
         <f t="shared" si="47"/>
         <v>135</v>
       </c>
-      <c r="N1020" s="37" t="s">
+      <c r="N1020" s="68" t="s">
         <v>1700</v>
       </c>
       <c r="O1020" s="6" t="s">
@@ -43130,7 +43171,7 @@
         <f t="shared" si="47"/>
         <v>138</v>
       </c>
-      <c r="N1023" s="37" t="s">
+      <c r="N1023" s="68" t="s">
         <v>304</v>
       </c>
       <c r="O1023" s="6"/>
@@ -43167,7 +43208,7 @@
         <f t="shared" si="47"/>
         <v>139</v>
       </c>
-      <c r="N1024" s="37" t="s">
+      <c r="N1024" s="68" t="s">
         <v>748</v>
       </c>
       <c r="O1024" s="5"/>
@@ -45131,7 +45172,7 @@
         <f t="shared" si="50"/>
         <v>199</v>
       </c>
-      <c r="N1084" s="37" t="s">
+      <c r="N1084" s="68" t="s">
         <v>232</v>
       </c>
       <c r="O1084" s="5" t="s">
@@ -45167,7 +45208,7 @@
         <f t="shared" si="50"/>
         <v>200</v>
       </c>
-      <c r="N1085" s="37" t="s">
+      <c r="N1085" s="68" t="s">
         <v>782</v>
       </c>
       <c r="O1085" s="5"/>
@@ -45643,7 +45684,7 @@
         <v>117</v>
       </c>
       <c r="T1099" s="6" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
       <c r="U1099" s="6"/>
       <c r="V1099" s="37"/>
@@ -47009,7 +47050,7 @@
         <f t="shared" si="53"/>
         <v>256</v>
       </c>
-      <c r="N1141" s="37" t="s">
+      <c r="N1141" s="68" t="s">
         <v>814</v>
       </c>
       <c r="O1141" s="5"/>
@@ -47045,7 +47086,7 @@
         <f t="shared" si="53"/>
         <v>257</v>
       </c>
-      <c r="N1142" s="37" t="s">
+      <c r="N1142" s="68" t="s">
         <v>233</v>
       </c>
       <c r="O1142" s="5"/>
@@ -48629,7 +48670,7 @@
         <f t="shared" si="56"/>
         <v>304</v>
       </c>
-      <c r="N1189" s="37" t="s">
+      <c r="N1189" s="68" t="s">
         <v>843</v>
       </c>
       <c r="O1189" s="5"/>
@@ -48665,7 +48706,7 @@
         <f t="shared" si="56"/>
         <v>305</v>
       </c>
-      <c r="N1190" s="37" t="s">
+      <c r="N1190" s="68" t="s">
         <v>844</v>
       </c>
       <c r="O1190" s="5"/>
@@ -49126,7 +49167,7 @@
         <f t="shared" si="56"/>
         <v>319</v>
       </c>
-      <c r="N1204" s="37" t="s">
+      <c r="N1204" s="68" t="s">
         <v>852</v>
       </c>
       <c r="O1204" s="5"/>
@@ -49159,7 +49200,7 @@
         <f t="shared" si="56"/>
         <v>320</v>
       </c>
-      <c r="N1205" s="37" t="s">
+      <c r="N1205" s="68" t="s">
         <v>853</v>
       </c>
       <c r="O1205" s="5"/>
@@ -49204,7 +49245,7 @@
     </row>
     <row r="1207" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1207" s="6" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="I1207" s="39" t="s">
         <v>46</v>
@@ -49929,7 +49970,7 @@
         <f t="shared" si="59"/>
         <v>22</v>
       </c>
-      <c r="N1229" s="37" t="s">
+      <c r="N1229" s="68" t="s">
         <v>270</v>
       </c>
       <c r="O1229" s="5"/>
@@ -49965,7 +50006,7 @@
         <f t="shared" si="59"/>
         <v>23</v>
       </c>
-      <c r="N1230" s="37" t="s">
+      <c r="N1230" s="68" t="s">
         <v>864</v>
       </c>
       <c r="O1230" s="6" t="s">
@@ -50922,7 +50963,7 @@
         <f t="shared" si="59"/>
         <v>52</v>
       </c>
-      <c r="N1259" s="37" t="s">
+      <c r="N1259" s="68" t="s">
         <v>879</v>
       </c>
       <c r="O1259" s="5"/>
@@ -50955,7 +50996,7 @@
         <f t="shared" si="59"/>
         <v>53</v>
       </c>
-      <c r="N1260" s="37" t="s">
+      <c r="N1260" s="68" t="s">
         <v>597</v>
       </c>
       <c r="O1260" s="5"/>
@@ -52168,7 +52209,7 @@
         <f t="shared" si="62"/>
         <v>90</v>
       </c>
-      <c r="N1297" s="37" t="s">
+      <c r="N1297" s="68" t="s">
         <v>1729</v>
       </c>
       <c r="O1297" s="6" t="s">
@@ -52640,10 +52681,10 @@
       <c r="Q1311" s="6"/>
       <c r="R1311" s="6"/>
       <c r="S1311" s="6" t="s">
+        <v>2074</v>
+      </c>
+      <c r="T1311" s="6" t="s">
         <v>2075</v>
-      </c>
-      <c r="T1311" s="6" t="s">
-        <v>2076</v>
       </c>
       <c r="U1311" s="6"/>
       <c r="V1311" s="37"/>
@@ -52707,7 +52748,7 @@
         <f t="shared" si="62"/>
         <v>106</v>
       </c>
-      <c r="N1313" s="37" t="s">
+      <c r="N1313" s="68" t="s">
         <v>907</v>
       </c>
       <c r="O1313" s="5"/>
@@ -52744,7 +52785,7 @@
         <f t="shared" si="62"/>
         <v>107</v>
       </c>
-      <c r="N1314" s="37" t="s">
+      <c r="N1314" s="68" t="s">
         <v>597</v>
       </c>
       <c r="O1314" s="5"/>
@@ -54399,8 +54440,8 @@
         <f t="shared" si="65"/>
         <v>156</v>
       </c>
-      <c r="N1363" s="37" t="s">
-        <v>2077</v>
+      <c r="N1363" s="68" t="s">
+        <v>2076</v>
       </c>
       <c r="O1363" s="6" t="s">
         <v>0</v>
@@ -55383,7 +55424,7 @@
         <f t="shared" si="65"/>
         <v>185</v>
       </c>
-      <c r="N1392" s="37" t="s">
+      <c r="N1392" s="68" t="s">
         <v>943</v>
       </c>
       <c r="O1392" s="6"/>
@@ -55417,7 +55458,7 @@
         <f t="shared" si="65"/>
         <v>186</v>
       </c>
-      <c r="N1393" s="37" t="s">
+      <c r="N1393" s="68" t="s">
         <v>1738</v>
       </c>
       <c r="O1393" s="6" t="s">
@@ -55861,7 +55902,7 @@
         <f t="shared" si="65"/>
         <v>199</v>
       </c>
-      <c r="N1406" s="37" t="s">
+      <c r="N1406" s="68" t="s">
         <v>1740</v>
       </c>
       <c r="O1406" s="5"/>
@@ -56071,7 +56112,7 @@
       <c r="N1412" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="O1412" s="58" t="s">
+      <c r="O1412" s="56" t="s">
         <v>1</v>
       </c>
       <c r="P1412" s="11" t="s">
@@ -56170,7 +56211,7 @@
         <f t="shared" si="68"/>
         <v>208</v>
       </c>
-      <c r="N1415" s="37" t="s">
+      <c r="N1415" s="68" t="s">
         <v>202</v>
       </c>
       <c r="O1415" s="5"/>
@@ -56204,7 +56245,7 @@
         <f t="shared" si="68"/>
         <v>209</v>
       </c>
-      <c r="N1416" s="37" t="s">
+      <c r="N1416" s="68" t="s">
         <v>950</v>
       </c>
       <c r="O1416" s="6" t="s">
@@ -56525,7 +56566,7 @@
       <c r="N1425" s="37" t="s">
         <v>349</v>
       </c>
-      <c r="O1425" s="58" t="s">
+      <c r="O1425" s="56" t="s">
         <v>1</v>
       </c>
       <c r="P1425" s="11" t="s">
@@ -56625,7 +56666,7 @@
         <v>221</v>
       </c>
       <c r="N1428" s="37" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
       <c r="O1428" s="5"/>
       <c r="P1428" s="6"/>
@@ -58168,7 +58209,7 @@
     </row>
     <row r="1475" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1475" s="6" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
       <c r="C1475" s="35"/>
       <c r="H1475" s="30"/>
@@ -58654,7 +58695,7 @@
         <f t="shared" si="71"/>
         <v>14</v>
       </c>
-      <c r="N1489" s="37" t="s">
+      <c r="N1489" s="68" t="s">
         <v>535</v>
       </c>
       <c r="O1489" s="5"/>
@@ -59149,7 +59190,7 @@
         <f t="shared" si="71"/>
         <v>29</v>
       </c>
-      <c r="N1504" s="37" t="s">
+      <c r="N1504" s="68" t="s">
         <v>214</v>
       </c>
       <c r="O1504" s="5"/>
@@ -59183,7 +59224,7 @@
         <f t="shared" si="71"/>
         <v>30</v>
       </c>
-      <c r="N1505" s="37" t="s">
+      <c r="N1505" s="68" t="s">
         <v>985</v>
       </c>
       <c r="O1505" s="6"/>
@@ -60583,7 +60624,7 @@
         <f t="shared" si="74"/>
         <v>72</v>
       </c>
-      <c r="N1547" s="37" t="s">
+      <c r="N1547" s="68" t="s">
         <v>1001</v>
       </c>
       <c r="O1547" s="5"/>
@@ -60616,7 +60657,7 @@
         <f t="shared" si="74"/>
         <v>73</v>
       </c>
-      <c r="N1548" s="37" t="s">
+      <c r="N1548" s="68" t="s">
         <v>1755</v>
       </c>
       <c r="O1548" s="6" t="s">
@@ -60909,7 +60950,7 @@
         <f t="shared" si="74"/>
         <v>82</v>
       </c>
-      <c r="N1557" s="37" t="s">
+      <c r="N1557" s="68" t="s">
         <v>255</v>
       </c>
       <c r="O1557" s="5"/>
@@ -61008,7 +61049,7 @@
         <f t="shared" si="74"/>
         <v>85</v>
       </c>
-      <c r="N1560" s="37" t="s">
+      <c r="N1560" s="68" t="s">
         <v>1010</v>
       </c>
       <c r="O1560" s="5" t="s">
@@ -61045,7 +61086,7 @@
         <f t="shared" si="74"/>
         <v>86</v>
       </c>
-      <c r="N1561" s="37" t="s">
+      <c r="N1561" s="68" t="s">
         <v>1011</v>
       </c>
       <c r="O1561" s="5"/>
@@ -62041,7 +62082,7 @@
         <v>118</v>
       </c>
       <c r="N1593" s="37" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
       <c r="O1593" s="6" t="s">
         <v>0</v>
@@ -62096,7 +62137,7 @@
         <f t="shared" si="74"/>
         <v>120</v>
       </c>
-      <c r="N1595" s="55" t="s">
+      <c r="N1595" s="53" t="s">
         <v>1032</v>
       </c>
       <c r="V1595" s="37"/>
@@ -63583,7 +63624,7 @@
         <f t="shared" si="77"/>
         <v>177</v>
       </c>
-      <c r="N1652" s="37" t="s">
+      <c r="N1652" s="68" t="s">
         <v>472</v>
       </c>
       <c r="S1652" s="1" t="s">
@@ -63619,7 +63660,7 @@
         <f t="shared" si="77"/>
         <v>178</v>
       </c>
-      <c r="N1653" s="37" t="s">
+      <c r="N1653" s="68" t="s">
         <v>831</v>
       </c>
       <c r="V1653" s="37"/>
@@ -63721,7 +63762,7 @@
         <f t="shared" si="77"/>
         <v>182</v>
       </c>
-      <c r="N1657" s="37" t="s">
+      <c r="N1657" s="68" t="s">
         <v>1763</v>
       </c>
       <c r="O1657" s="6" t="s">
@@ -63730,7 +63771,7 @@
       <c r="P1657" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="U1657" s="1" t="s">
+      <c r="U1657" s="6" t="s">
         <v>94</v>
       </c>
       <c r="V1657" s="37" t="s">
@@ -63762,6 +63803,7 @@
       <c r="O1658" s="6" t="s">
         <v>0</v>
       </c>
+      <c r="U1658" s="6"/>
       <c r="V1658" s="37" t="s">
         <v>1560</v>
       </c>
@@ -63788,7 +63830,7 @@
       <c r="N1659" s="37" t="s">
         <v>1067</v>
       </c>
-      <c r="U1659" s="1" t="s">
+      <c r="U1659" s="6" t="s">
         <v>173</v>
       </c>
       <c r="V1659" s="37"/>
@@ -64168,7 +64210,7 @@
         <f t="shared" si="80"/>
         <v>9</v>
       </c>
-      <c r="N1673" s="37" t="s">
+      <c r="N1673" s="68" t="s">
         <v>720</v>
       </c>
       <c r="V1673" s="37"/>
@@ -64195,7 +64237,7 @@
         <f t="shared" si="80"/>
         <v>10</v>
       </c>
-      <c r="N1674" s="37" t="s">
+      <c r="N1674" s="68" t="s">
         <v>472</v>
       </c>
       <c r="S1674" s="1" t="s">
@@ -64579,7 +64621,7 @@
         <f t="shared" si="80"/>
         <v>24</v>
       </c>
-      <c r="N1688" s="37" t="s">
+      <c r="N1688" s="68" t="s">
         <v>1078</v>
       </c>
       <c r="U1688" s="1" t="s">
@@ -65162,7 +65204,7 @@
         <f t="shared" si="80"/>
         <v>47</v>
       </c>
-      <c r="N1711" s="37" t="s">
+      <c r="N1711" s="68" t="s">
         <v>1090</v>
       </c>
       <c r="U1711" s="1" t="s">
@@ -65902,7 +65944,7 @@
         <f t="shared" si="83"/>
         <v>75</v>
       </c>
-      <c r="N1739" s="37" t="s">
+      <c r="N1739" s="68" t="s">
         <v>1106</v>
       </c>
       <c r="U1739" s="1" t="s">
@@ -66077,7 +66119,7 @@
         <f t="shared" si="83"/>
         <v>81</v>
       </c>
-      <c r="N1745" s="37" t="s">
+      <c r="N1745" s="68" t="s">
         <v>417</v>
       </c>
       <c r="U1745" s="1" t="s">
@@ -66159,7 +66201,7 @@
         <v>90</v>
       </c>
       <c r="T1748" s="1" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
       <c r="V1748" s="37"/>
     </row>
@@ -66467,7 +66509,7 @@
         <v>1968</v>
       </c>
     </row>
-    <row r="1761" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1761" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1761" s="39" t="s">
         <v>57</v>
       </c>
@@ -66491,7 +66533,7 @@
       </c>
       <c r="V1761" s="37"/>
     </row>
-    <row r="1762" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1762" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1762" s="39" t="s">
         <v>57</v>
       </c>
@@ -66515,7 +66557,7 @@
       </c>
       <c r="V1762" s="37"/>
     </row>
-    <row r="1763" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1763" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1763" s="39" t="s">
         <v>57</v>
       </c>
@@ -66539,7 +66581,7 @@
       </c>
       <c r="V1763" s="37"/>
     </row>
-    <row r="1764" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1764" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1764" s="39" t="s">
         <v>57</v>
       </c>
@@ -66566,7 +66608,7 @@
       </c>
       <c r="V1764" s="37"/>
     </row>
-    <row r="1765" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1765" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="H1765" s="44" t="s">
         <v>155</v>
       </c>
@@ -66592,7 +66634,7 @@
       </c>
       <c r="V1765" s="37"/>
     </row>
-    <row r="1766" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1766" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="H1766" s="44" t="s">
         <v>155</v>
       </c>
@@ -66619,7 +66661,7 @@
       </c>
       <c r="V1766" s="37"/>
     </row>
-    <row r="1767" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1767" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="H1767" s="44" t="s">
         <v>155</v>
       </c>
@@ -66646,7 +66688,7 @@
       </c>
       <c r="V1767" s="37"/>
     </row>
-    <row r="1768" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1768" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="H1768" s="44" t="s">
         <v>155</v>
       </c>
@@ -66673,7 +66715,10 @@
       </c>
       <c r="V1768" s="37"/>
     </row>
-    <row r="1769" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1769" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A1769" s="6" t="s">
+        <v>2087</v>
+      </c>
       <c r="H1769" s="44" t="s">
         <v>155</v>
       </c>
@@ -66695,7 +66740,7 @@
         <f t="shared" si="83"/>
         <v>105</v>
       </c>
-      <c r="N1769" s="55" t="s">
+      <c r="N1769" s="68" t="s">
         <v>195</v>
       </c>
       <c r="O1769" s="5" t="s">
@@ -66703,7 +66748,7 @@
       </c>
       <c r="V1769" s="37"/>
     </row>
-    <row r="1770" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1770" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="H1770" s="44" t="s">
         <v>155</v>
       </c>
@@ -66725,12 +66770,12 @@
         <f t="shared" si="83"/>
         <v>106</v>
       </c>
-      <c r="N1770" s="37" t="s">
+      <c r="N1770" s="68" t="s">
         <v>418</v>
       </c>
       <c r="V1770" s="37"/>
     </row>
-    <row r="1771" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1771" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="H1771" s="44" t="s">
         <v>155</v>
       </c>
@@ -66757,7 +66802,7 @@
       </c>
       <c r="V1771" s="37"/>
     </row>
-    <row r="1772" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1772" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="H1772" s="44" t="s">
         <v>155</v>
       </c>
@@ -66789,7 +66834,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="1773" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1773" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1773" s="39" t="s">
         <v>58</v>
       </c>
@@ -66813,7 +66858,7 @@
       </c>
       <c r="V1773" s="37"/>
     </row>
-    <row r="1774" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1774" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1774" s="39" t="s">
         <v>58</v>
       </c>
@@ -66837,7 +66882,7 @@
       </c>
       <c r="V1774" s="37"/>
     </row>
-    <row r="1775" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1775" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1775" s="39" t="s">
         <v>58</v>
       </c>
@@ -66864,7 +66909,7 @@
       </c>
       <c r="V1775" s="37"/>
     </row>
-    <row r="1776" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1776" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1776" s="39" t="s">
         <v>58</v>
       </c>
@@ -67064,7 +67109,7 @@
         <f t="shared" si="83"/>
         <v>119</v>
       </c>
-      <c r="N1783" s="37" t="s">
+      <c r="N1783" s="68" t="s">
         <v>602</v>
       </c>
       <c r="U1783" s="1" t="s">
@@ -67091,7 +67136,7 @@
         <f t="shared" si="83"/>
         <v>120</v>
       </c>
-      <c r="N1784" s="37" t="s">
+      <c r="N1784" s="68" t="s">
         <v>1118</v>
       </c>
       <c r="V1784" s="37"/>
@@ -67214,7 +67259,7 @@
       <c r="N1789" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="O1789" s="58" t="s">
+      <c r="O1789" s="56" t="s">
         <v>1</v>
       </c>
       <c r="P1789" s="11" t="s">
@@ -67243,7 +67288,7 @@
         <f t="shared" si="83"/>
         <v>126</v>
       </c>
-      <c r="N1790" s="37" t="s">
+      <c r="N1790" s="68" t="s">
         <v>578</v>
       </c>
       <c r="V1790" s="37"/>
@@ -67267,7 +67312,7 @@
         <f t="shared" si="83"/>
         <v>127</v>
       </c>
-      <c r="N1791" s="37" t="s">
+      <c r="N1791" s="68" t="s">
         <v>1120</v>
       </c>
       <c r="U1791" s="1" t="s">
@@ -67294,7 +67339,7 @@
         <f t="shared" si="83"/>
         <v>128</v>
       </c>
-      <c r="N1792" s="37" t="s">
+      <c r="N1792" s="68" t="s">
         <v>578</v>
       </c>
       <c r="V1792" s="37"/>
@@ -67664,7 +67709,7 @@
         <f t="shared" si="86"/>
         <v>142</v>
       </c>
-      <c r="N1806" s="37" t="s">
+      <c r="N1806" s="68" t="s">
         <v>354</v>
       </c>
       <c r="O1806" s="6" t="s">
@@ -67696,7 +67741,7 @@
         <f t="shared" si="86"/>
         <v>143</v>
       </c>
-      <c r="N1807" s="37" t="s">
+      <c r="N1807" s="68" t="s">
         <v>1124</v>
       </c>
       <c r="V1807" s="37"/>
@@ -67979,7 +68024,7 @@
       <c r="N1818" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="O1818" s="59" t="s">
+      <c r="O1818" s="57" t="s">
         <v>1</v>
       </c>
       <c r="P1818" s="11" t="s">
@@ -68135,7 +68180,7 @@
     </row>
     <row r="1825" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1825" s="6" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
       <c r="I1825" s="39" t="s">
         <v>58</v>
@@ -69881,7 +69926,7 @@
       <c r="N1893" s="37" t="s">
         <v>349</v>
       </c>
-      <c r="O1893" s="58" t="s">
+      <c r="O1893" s="56" t="s">
         <v>1</v>
       </c>
       <c r="P1893" s="11" t="s">
@@ -71316,7 +71361,7 @@
         <f t="shared" si="92"/>
         <v>124</v>
       </c>
-      <c r="N1949" s="37" t="s">
+      <c r="N1949" s="68" t="s">
         <v>602</v>
       </c>
       <c r="U1949" s="1" t="s">
@@ -71343,7 +71388,7 @@
         <f t="shared" si="92"/>
         <v>125</v>
       </c>
-      <c r="N1950" s="37" t="s">
+      <c r="N1950" s="68" t="s">
         <v>233</v>
       </c>
       <c r="V1950" s="37"/>
@@ -72492,7 +72537,7 @@
         <f t="shared" si="95"/>
         <v>170</v>
       </c>
-      <c r="N1995" s="37" t="s">
+      <c r="N1995" s="68" t="s">
         <v>242</v>
       </c>
       <c r="V1995" s="37"/>
@@ -72516,10 +72561,10 @@
         <f t="shared" si="95"/>
         <v>171</v>
       </c>
-      <c r="N1996" s="37" t="s">
+      <c r="N1996" s="68" t="s">
         <v>255</v>
       </c>
-      <c r="T1996" s="1" t="s">
+      <c r="U1996" s="1" t="s">
         <v>186</v>
       </c>
       <c r="V1996" s="37"/>
@@ -72543,7 +72588,7 @@
         <f t="shared" si="95"/>
         <v>172</v>
       </c>
-      <c r="N1997" s="37" t="s">
+      <c r="N1997" s="68" t="s">
         <v>436</v>
       </c>
       <c r="V1997" s="37"/>
@@ -73135,7 +73180,7 @@
         <v>195</v>
       </c>
       <c r="N2020" s="37" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="V2020" s="37"/>
     </row>
@@ -73889,7 +73934,7 @@
       </c>
       <c r="V2048" s="37"/>
     </row>
-    <row r="2049" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2049" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="H2049" s="44" t="s">
         <v>158</v>
       </c>
@@ -73911,7 +73956,7 @@
         <f t="shared" si="95"/>
         <v>224</v>
       </c>
-      <c r="N2049" s="37" t="s">
+      <c r="N2049" s="68" t="s">
         <v>255</v>
       </c>
       <c r="U2049" s="1" t="s">
@@ -73919,7 +73964,7 @@
       </c>
       <c r="V2049" s="37"/>
     </row>
-    <row r="2050" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2050" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="H2050" s="44" t="s">
         <v>158</v>
       </c>
@@ -73946,7 +73991,7 @@
       </c>
       <c r="V2050" s="37"/>
     </row>
-    <row r="2051" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2051" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="H2051" s="44" t="s">
         <v>158</v>
       </c>
@@ -73978,7 +74023,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2052" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2052" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2052" s="39" t="s">
         <v>63</v>
       </c>
@@ -74005,7 +74050,7 @@
       </c>
       <c r="V2052" s="37"/>
     </row>
-    <row r="2053" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2053" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2053" s="39" t="s">
         <v>63</v>
       </c>
@@ -74029,7 +74074,7 @@
       </c>
       <c r="V2053" s="37"/>
     </row>
-    <row r="2054" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2054" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2054" s="39" t="s">
         <v>63</v>
       </c>
@@ -74053,7 +74098,7 @@
       </c>
       <c r="V2054" s="37"/>
     </row>
-    <row r="2055" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2055" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2055" s="39" t="s">
         <v>63</v>
       </c>
@@ -74082,7 +74127,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="2056" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2056" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2056" s="39" t="s">
         <v>63</v>
       </c>
@@ -74106,7 +74151,7 @@
       </c>
       <c r="V2056" s="37"/>
     </row>
-    <row r="2057" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2057" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2057" s="39" t="s">
         <v>63</v>
       </c>
@@ -74130,7 +74175,7 @@
       </c>
       <c r="V2057" s="37"/>
     </row>
-    <row r="2058" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2058" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2058" s="39" t="s">
         <v>63</v>
       </c>
@@ -74154,7 +74199,7 @@
       </c>
       <c r="V2058" s="37"/>
     </row>
-    <row r="2059" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2059" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2059" s="39" t="s">
         <v>63</v>
       </c>
@@ -74181,7 +74226,7 @@
       </c>
       <c r="V2059" s="37"/>
     </row>
-    <row r="2060" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2060" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2060" s="39" t="s">
         <v>63</v>
       </c>
@@ -74205,7 +74250,7 @@
       </c>
       <c r="V2060" s="37"/>
     </row>
-    <row r="2061" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2061" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2061" s="39" t="s">
         <v>63</v>
       </c>
@@ -74229,7 +74274,7 @@
       </c>
       <c r="V2061" s="37"/>
     </row>
-    <row r="2062" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2062" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2062" s="39" t="s">
         <v>63</v>
       </c>
@@ -74253,7 +74298,7 @@
       </c>
       <c r="V2062" s="37"/>
     </row>
-    <row r="2063" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2063" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2063" s="39" t="s">
         <v>63</v>
       </c>
@@ -74277,7 +74322,12 @@
       </c>
       <c r="V2063" s="37"/>
     </row>
-    <row r="2064" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2064" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A2064" s="69" t="s">
+        <v>2088</v>
+      </c>
+      <c r="B2064" s="70"/>
+      <c r="C2064" s="71"/>
       <c r="I2064" s="39" t="s">
         <v>63</v>
       </c>
@@ -74296,14 +74346,11 @@
         <f t="shared" si="98"/>
         <v>239</v>
       </c>
-      <c r="N2064" s="37" t="s">
+      <c r="N2064" s="72" t="s">
         <v>195</v>
       </c>
       <c r="O2064" s="5" t="s">
         <v>1</v>
-      </c>
-      <c r="U2064" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="V2064" s="37"/>
     </row>
@@ -74326,7 +74373,7 @@
         <f t="shared" si="98"/>
         <v>240</v>
       </c>
-      <c r="N2065" s="37" t="s">
+      <c r="N2065" s="72" t="s">
         <v>418</v>
       </c>
       <c r="V2065" s="37"/>
@@ -76298,7 +76345,7 @@
         <f t="shared" si="101"/>
         <v>12</v>
       </c>
-      <c r="N2141" s="37" t="s">
+      <c r="N2141" s="68" t="s">
         <v>232</v>
       </c>
       <c r="O2141" s="5" t="s">
@@ -76331,7 +76378,7 @@
         <f t="shared" si="101"/>
         <v>13</v>
       </c>
-      <c r="N2142" s="37" t="s">
+      <c r="N2142" s="68" t="s">
         <v>1251</v>
       </c>
       <c r="V2142" s="37"/>
@@ -76728,7 +76775,7 @@
         <f t="shared" si="101"/>
         <v>28</v>
       </c>
-      <c r="N2157" s="37" t="s">
+      <c r="N2157" s="68" t="s">
         <v>195</v>
       </c>
       <c r="O2157" s="5" t="s">
@@ -76758,7 +76805,7 @@
         <f t="shared" si="101"/>
         <v>29</v>
       </c>
-      <c r="N2158" s="37" t="s">
+      <c r="N2158" s="68" t="s">
         <v>242</v>
       </c>
       <c r="V2158" s="37"/>
@@ -77630,7 +77677,7 @@
         <f t="shared" si="103"/>
         <v>63</v>
       </c>
-      <c r="N2192" s="37" t="s">
+      <c r="N2192" s="68" t="s">
         <v>195</v>
       </c>
       <c r="O2192" s="5" t="s">
@@ -77660,7 +77707,7 @@
         <f t="shared" si="103"/>
         <v>64</v>
       </c>
-      <c r="N2193" s="37" t="s">
+      <c r="N2193" s="68" t="s">
         <v>242</v>
       </c>
       <c r="V2193" s="37"/>
@@ -77938,7 +77985,7 @@
         <f t="shared" si="103"/>
         <v>75</v>
       </c>
-      <c r="N2204" s="37" t="s">
+      <c r="N2204" s="68" t="s">
         <v>405</v>
       </c>
       <c r="U2204" s="1" t="s">
@@ -77965,7 +78012,7 @@
         <f t="shared" si="103"/>
         <v>76</v>
       </c>
-      <c r="N2205" s="37" t="s">
+      <c r="N2205" s="68" t="s">
         <v>1279</v>
       </c>
       <c r="V2205" s="37"/>
@@ -78738,7 +78785,7 @@
         <f t="shared" si="103"/>
         <v>106</v>
       </c>
-      <c r="N2235" s="37" t="s">
+      <c r="N2235" s="68" t="s">
         <v>195</v>
       </c>
       <c r="O2235" s="5" t="s">
@@ -78768,7 +78815,7 @@
         <f t="shared" si="103"/>
         <v>107</v>
       </c>
-      <c r="N2236" s="37" t="s">
+      <c r="N2236" s="68" t="s">
         <v>242</v>
       </c>
       <c r="V2236" s="37"/>
@@ -79853,7 +79900,7 @@
         <f t="shared" si="107"/>
         <v>150</v>
       </c>
-      <c r="N2279" s="37" t="s">
+      <c r="N2279" s="68" t="s">
         <v>195</v>
       </c>
       <c r="O2279" s="5" t="s">
@@ -79882,7 +79929,7 @@
         <f t="shared" si="107"/>
         <v>151</v>
       </c>
-      <c r="N2280" s="37" t="s">
+      <c r="N2280" s="68" t="s">
         <v>242</v>
       </c>
       <c r="V2280" s="37"/>
@@ -80178,7 +80225,7 @@
         <f t="shared" si="107"/>
         <v>162</v>
       </c>
-      <c r="N2291" s="37" t="s">
+      <c r="N2291" s="68" t="s">
         <v>288</v>
       </c>
       <c r="O2291" s="5" t="s">
@@ -80211,7 +80258,7 @@
         <f t="shared" si="107"/>
         <v>163</v>
       </c>
-      <c r="N2292" s="37" t="s">
+      <c r="N2292" s="68" t="s">
         <v>298</v>
       </c>
       <c r="V2292" s="37"/>
@@ -80358,7 +80405,7 @@
       <c r="N2298" s="37" t="s">
         <v>349</v>
       </c>
-      <c r="O2298" s="58" t="s">
+      <c r="O2298" s="56" t="s">
         <v>1</v>
       </c>
       <c r="P2298" s="11" t="s">
@@ -80522,7 +80569,7 @@
         <f t="shared" si="107"/>
         <v>175</v>
       </c>
-      <c r="N2304" s="37" t="s">
+      <c r="N2304" s="68" t="s">
         <v>255</v>
       </c>
       <c r="U2304" s="1" t="s">
@@ -80549,7 +80596,7 @@
         <f t="shared" si="107"/>
         <v>176</v>
       </c>
-      <c r="N2305" s="37" t="s">
+      <c r="N2305" s="68" t="s">
         <v>1307</v>
       </c>
       <c r="V2305" s="37"/>
@@ -80887,7 +80934,7 @@
         <f t="shared" si="110"/>
         <v>189</v>
       </c>
-      <c r="N2318" s="37" t="s">
+      <c r="N2318" s="68" t="s">
         <v>417</v>
       </c>
       <c r="P2318" s="11" t="s">
@@ -81114,7 +81161,7 @@
         <f t="shared" si="110"/>
         <v>198</v>
       </c>
-      <c r="N2327" s="37" t="s">
+      <c r="N2327" s="68" t="s">
         <v>417</v>
       </c>
       <c r="U2327" s="1" t="s">
@@ -81218,7 +81265,7 @@
         <f t="shared" si="110"/>
         <v>202</v>
       </c>
-      <c r="N2331" s="37" t="s">
+      <c r="N2331" s="68" t="s">
         <v>195</v>
       </c>
       <c r="O2331" s="5" t="s">
@@ -81248,7 +81295,7 @@
         <f t="shared" si="110"/>
         <v>203</v>
       </c>
-      <c r="N2332" s="37" t="s">
+      <c r="N2332" s="68" t="s">
         <v>242</v>
       </c>
       <c r="V2332" s="37"/>
@@ -81378,7 +81425,7 @@
     </row>
     <row r="2338" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2338" s="6" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="I2338" s="39" t="s">
         <v>68</v>
@@ -83524,7 +83571,7 @@
         <f t="shared" si="113"/>
         <v>79</v>
       </c>
-      <c r="N2417" s="37" t="s">
+      <c r="N2417" s="68" t="s">
         <v>1356</v>
       </c>
       <c r="V2417" s="37"/>
@@ -83548,7 +83595,7 @@
         <f t="shared" si="113"/>
         <v>80</v>
       </c>
-      <c r="N2418" s="37" t="s">
+      <c r="N2418" s="68" t="s">
         <v>1357</v>
       </c>
       <c r="U2418" s="1" t="s">
@@ -83575,7 +83622,7 @@
         <f t="shared" si="113"/>
         <v>81</v>
       </c>
-      <c r="N2419" s="37" t="s">
+      <c r="N2419" s="68" t="s">
         <v>1358</v>
       </c>
       <c r="V2419" s="37"/>
@@ -84130,7 +84177,7 @@
         <f t="shared" si="116"/>
         <v>102</v>
       </c>
-      <c r="N2440" s="37" t="s">
+      <c r="N2440" s="68" t="s">
         <v>419</v>
       </c>
       <c r="U2440" s="1" t="s">
@@ -84157,7 +84204,7 @@
         <f t="shared" si="116"/>
         <v>103</v>
       </c>
-      <c r="N2441" s="37" t="s">
+      <c r="N2441" s="68" t="s">
         <v>1367</v>
       </c>
       <c r="V2441" s="37"/>
@@ -84695,7 +84742,7 @@
       <c r="N2461" s="37" t="s">
         <v>1379</v>
       </c>
-      <c r="O2461" s="60"/>
+      <c r="O2461" s="6"/>
       <c r="V2461" s="37"/>
     </row>
     <row r="2462" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -84784,7 +84831,7 @@
         <v>2054</v>
       </c>
     </row>
-    <row r="2465" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2465" spans="1:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2465" s="39" t="s">
         <v>71</v>
       </c>
@@ -84803,7 +84850,7 @@
         <f t="shared" si="116"/>
         <v>127</v>
       </c>
-      <c r="N2465" s="37" t="s">
+      <c r="N2465" s="68" t="s">
         <v>354</v>
       </c>
       <c r="O2465" s="6" t="s">
@@ -84816,7 +84863,7 @@
         <v>1413</v>
       </c>
     </row>
-    <row r="2466" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2466" spans="1:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2466" s="39" t="s">
         <v>71</v>
       </c>
@@ -84835,7 +84882,7 @@
         <f t="shared" si="116"/>
         <v>128</v>
       </c>
-      <c r="N2466" s="37" t="s">
+      <c r="N2466" s="68" t="s">
         <v>255</v>
       </c>
       <c r="U2466" s="1" t="s">
@@ -84843,7 +84890,7 @@
       </c>
       <c r="V2466" s="37"/>
     </row>
-    <row r="2467" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2467" spans="1:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2467" s="39" t="s">
         <v>71</v>
       </c>
@@ -84873,7 +84920,7 @@
       </c>
       <c r="V2467" s="37"/>
     </row>
-    <row r="2468" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2468" spans="1:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2468" s="39" t="s">
         <v>71</v>
       </c>
@@ -84899,9 +84946,9 @@
       <c r="T2468" s="6"/>
       <c r="V2468" s="37"/>
     </row>
-    <row r="2469" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2469" spans="1:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2469" s="6" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
       <c r="I2469" s="39" t="s">
         <v>71</v>
@@ -84921,14 +84968,17 @@
         <f t="shared" si="116"/>
         <v>131</v>
       </c>
-      <c r="N2469" s="55" t="s">
+      <c r="N2469" s="53" t="s">
         <v>199</v>
       </c>
       <c r="S2469" s="6"/>
       <c r="T2469" s="6"/>
       <c r="V2469" s="37"/>
-    </row>
-    <row r="2470" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="X2469" s="6" t="s">
+        <v>2084</v>
+      </c>
+    </row>
+    <row r="2470" spans="1:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2470" s="39" t="s">
         <v>71</v>
       </c>
@@ -84947,14 +84997,14 @@
         <f t="shared" si="116"/>
         <v>132</v>
       </c>
-      <c r="N2470" s="55" t="s">
+      <c r="N2470" s="53" t="s">
         <v>526</v>
       </c>
       <c r="S2470" s="6"/>
       <c r="T2470" s="6"/>
       <c r="V2470" s="37"/>
     </row>
-    <row r="2471" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2471" spans="1:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2471" s="39" t="s">
         <v>71</v>
       </c>
@@ -84973,7 +85023,7 @@
         <f t="shared" si="116"/>
         <v>133</v>
       </c>
-      <c r="N2471" s="37" t="s">
+      <c r="N2471" s="68" t="s">
         <v>195</v>
       </c>
       <c r="O2471" s="5" t="s">
@@ -84986,7 +85036,7 @@
       </c>
       <c r="V2471" s="37"/>
     </row>
-    <row r="2472" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2472" spans="1:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2472" s="39" t="s">
         <v>71</v>
       </c>
@@ -85005,7 +85055,7 @@
         <f t="shared" si="116"/>
         <v>134</v>
       </c>
-      <c r="N2472" s="37" t="s">
+      <c r="N2472" s="68" t="s">
         <v>1672</v>
       </c>
       <c r="P2472" s="11" t="s">
@@ -85017,7 +85067,7 @@
         <v>2055</v>
       </c>
     </row>
-    <row r="2473" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2473" spans="1:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2473" s="39" t="s">
         <v>71</v>
       </c>
@@ -85043,7 +85093,7 @@
       <c r="T2473" s="6"/>
       <c r="V2473" s="37"/>
     </row>
-    <row r="2474" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2474" spans="1:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2474" s="39" t="s">
         <v>71</v>
       </c>
@@ -85069,7 +85119,7 @@
       <c r="T2474" s="6"/>
       <c r="V2474" s="37"/>
     </row>
-    <row r="2475" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2475" spans="1:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2475" s="39" t="s">
         <v>71</v>
       </c>
@@ -85095,7 +85145,7 @@
       <c r="T2475" s="6"/>
       <c r="V2475" s="37"/>
     </row>
-    <row r="2476" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2476" spans="1:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2476" s="39" t="s">
         <v>71</v>
       </c>
@@ -85124,13 +85174,13 @@
         <v>90</v>
       </c>
       <c r="T2476" s="6" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="V2476" s="37" t="s">
         <v>1876</v>
       </c>
     </row>
-    <row r="2477" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2477" spans="1:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2477" s="39" t="s">
         <v>71</v>
       </c>
@@ -85156,7 +85206,7 @@
       <c r="T2477" s="6"/>
       <c r="V2477" s="37"/>
     </row>
-    <row r="2478" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2478" spans="1:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2478" s="39" t="s">
         <v>71</v>
       </c>
@@ -85182,7 +85232,7 @@
       <c r="T2478" s="6"/>
       <c r="V2478" s="37"/>
     </row>
-    <row r="2479" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2479" spans="1:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2479" s="39" t="s">
         <v>71</v>
       </c>
@@ -85217,7 +85267,7 @@
         <v>1633</v>
       </c>
     </row>
-    <row r="2480" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2480" spans="1:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2480" s="39" t="s">
         <v>71</v>
       </c>
@@ -85591,7 +85641,7 @@
         <f t="shared" si="116"/>
         <v>156</v>
       </c>
-      <c r="N2494" s="37" t="s">
+      <c r="N2494" s="68" t="s">
         <v>233</v>
       </c>
       <c r="V2494" s="37"/>
@@ -85618,7 +85668,7 @@
         <f t="shared" si="116"/>
         <v>157</v>
       </c>
-      <c r="N2495" s="37" t="s">
+      <c r="N2495" s="68" t="s">
         <v>255</v>
       </c>
       <c r="U2495" s="1" t="s">
@@ -85648,7 +85698,7 @@
         <f t="shared" si="116"/>
         <v>158</v>
       </c>
-      <c r="N2496" s="37" t="s">
+      <c r="N2496" s="68" t="s">
         <v>199</v>
       </c>
       <c r="V2496" s="37"/>
@@ -85702,7 +85752,7 @@
         <f t="shared" si="116"/>
         <v>160</v>
       </c>
-      <c r="N2498" s="37" t="s">
+      <c r="N2498" s="68" t="s">
         <v>233</v>
       </c>
       <c r="V2498" s="37"/>
@@ -85729,7 +85779,7 @@
         <f t="shared" si="116"/>
         <v>161</v>
       </c>
-      <c r="N2499" s="37" t="s">
+      <c r="N2499" s="68" t="s">
         <v>255</v>
       </c>
       <c r="P2499" s="11" t="s">

</xml_diff>

<commit_message>
Update TS 4.2 Padam Input Template.xlsx
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.2 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.2 Padam Input Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D024890-01A5-4DE5-946C-51294751806C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F0537D-35EF-4936-8EDC-77DC6D2FAF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TS 4,2" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,18 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TS 4,2'!$A$1:$V$2500</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>

</xml_diff>

<commit_message>
nmv 05 01 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.2 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.2 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CA6F64-E914-4D95-A907-856E6405A5BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5D1571-55AE-4563-A710-DC19299BE4D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6525,7 +6525,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -6744,21 +6744,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -7044,9 +7029,9 @@
   <dimension ref="A1:X2500"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2484" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A624" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N2498" sqref="N2498"/>
+      <selection pane="bottomLeft" activeCell="N640" sqref="N640"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -30472,8 +30457,8 @@
       <c r="S640" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="T640" s="6" t="s">
-        <v>91</v>
+      <c r="T640" s="64" t="s">
+        <v>2058</v>
       </c>
       <c r="U640" s="6"/>
       <c r="V640" s="37"/>
@@ -49808,127 +49793,127 @@
       <c r="V1223" s="37"/>
     </row>
     <row r="1224" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I1224" s="76" t="s">
+      <c r="I1224" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="J1224" s="77">
+      <c r="J1224" s="38">
         <v>24</v>
       </c>
-      <c r="K1224" s="76">
+      <c r="K1224" s="39">
         <f t="shared" si="57"/>
         <v>1223</v>
       </c>
-      <c r="L1224" s="76">
+      <c r="L1224" s="39">
         <f t="shared" si="58"/>
         <v>17</v>
       </c>
-      <c r="M1224" s="76">
+      <c r="M1224" s="39">
         <f t="shared" si="59"/>
         <v>17</v>
       </c>
-      <c r="N1224" s="78" t="s">
+      <c r="N1224" s="37" t="s">
         <v>858</v>
       </c>
-      <c r="O1224" s="79"/>
-      <c r="P1224" s="80"/>
-      <c r="Q1224" s="80"/>
-      <c r="R1224" s="80"/>
-      <c r="S1224" s="80"/>
-      <c r="T1224" s="80"/>
-      <c r="U1224" s="80"/>
+      <c r="O1224" s="5"/>
+      <c r="P1224" s="6"/>
+      <c r="Q1224" s="6"/>
+      <c r="R1224" s="6"/>
+      <c r="S1224" s="6"/>
+      <c r="T1224" s="6"/>
+      <c r="U1224" s="6"/>
       <c r="V1224" s="37"/>
     </row>
     <row r="1225" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I1225" s="76" t="s">
+      <c r="I1225" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="J1225" s="77">
+      <c r="J1225" s="38">
         <v>24</v>
       </c>
-      <c r="K1225" s="76">
+      <c r="K1225" s="39">
         <f t="shared" si="57"/>
         <v>1224</v>
       </c>
-      <c r="L1225" s="76">
+      <c r="L1225" s="39">
         <f t="shared" si="58"/>
         <v>18</v>
       </c>
-      <c r="M1225" s="76">
+      <c r="M1225" s="39">
         <f t="shared" si="59"/>
         <v>18</v>
       </c>
-      <c r="N1225" s="78" t="s">
+      <c r="N1225" s="37" t="s">
         <v>245</v>
       </c>
-      <c r="O1225" s="79"/>
-      <c r="P1225" s="80"/>
-      <c r="Q1225" s="80"/>
-      <c r="R1225" s="80"/>
-      <c r="S1225" s="80"/>
-      <c r="T1225" s="80"/>
-      <c r="U1225" s="80"/>
+      <c r="O1225" s="5"/>
+      <c r="P1225" s="6"/>
+      <c r="Q1225" s="6"/>
+      <c r="R1225" s="6"/>
+      <c r="S1225" s="6"/>
+      <c r="T1225" s="6"/>
+      <c r="U1225" s="6"/>
       <c r="V1225" s="37"/>
     </row>
     <row r="1226" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I1226" s="76" t="s">
+      <c r="I1226" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="J1226" s="77">
+      <c r="J1226" s="38">
         <v>24</v>
       </c>
-      <c r="K1226" s="76">
+      <c r="K1226" s="39">
         <f t="shared" si="57"/>
         <v>1225</v>
       </c>
-      <c r="L1226" s="76">
+      <c r="L1226" s="39">
         <f t="shared" si="58"/>
         <v>19</v>
       </c>
-      <c r="M1226" s="76">
+      <c r="M1226" s="39">
         <f t="shared" si="59"/>
         <v>19</v>
       </c>
-      <c r="N1226" s="78" t="s">
+      <c r="N1226" s="37" t="s">
         <v>861</v>
       </c>
-      <c r="O1226" s="79"/>
-      <c r="P1226" s="80"/>
-      <c r="Q1226" s="80"/>
-      <c r="R1226" s="80"/>
-      <c r="S1226" s="80"/>
-      <c r="T1226" s="80"/>
-      <c r="U1226" s="80"/>
+      <c r="O1226" s="5"/>
+      <c r="P1226" s="6"/>
+      <c r="Q1226" s="6"/>
+      <c r="R1226" s="6"/>
+      <c r="S1226" s="6"/>
+      <c r="T1226" s="6"/>
+      <c r="U1226" s="6"/>
       <c r="V1226" s="37"/>
     </row>
     <row r="1227" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I1227" s="76" t="s">
+      <c r="I1227" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="J1227" s="77">
+      <c r="J1227" s="38">
         <v>24</v>
       </c>
-      <c r="K1227" s="76">
+      <c r="K1227" s="39">
         <f t="shared" si="57"/>
         <v>1226</v>
       </c>
-      <c r="L1227" s="76">
+      <c r="L1227" s="39">
         <f t="shared" si="58"/>
         <v>20</v>
       </c>
-      <c r="M1227" s="76">
+      <c r="M1227" s="39">
         <f t="shared" si="59"/>
         <v>20</v>
       </c>
-      <c r="N1227" s="78" t="s">
+      <c r="N1227" s="37" t="s">
         <v>595</v>
       </c>
-      <c r="O1227" s="79"/>
-      <c r="P1227" s="80"/>
-      <c r="Q1227" s="80"/>
-      <c r="R1227" s="80"/>
-      <c r="S1227" s="80"/>
-      <c r="T1227" s="80"/>
-      <c r="U1227" s="80"/>
+      <c r="O1227" s="5"/>
+      <c r="P1227" s="6"/>
+      <c r="Q1227" s="6"/>
+      <c r="R1227" s="6"/>
+      <c r="S1227" s="6"/>
+      <c r="T1227" s="6"/>
+      <c r="U1227" s="6"/>
       <c r="V1227" s="37"/>
     </row>
     <row r="1228" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
nmv 10 01 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.2 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.2 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5D1571-55AE-4563-A710-DC19299BE4D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08AF494-7240-4EC3-9C6F-683917448670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7029,9 +7029,9 @@
   <dimension ref="A1:X2500"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A624" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N640" sqref="N640"/>
+      <selection pane="bottomLeft" activeCell="U130" sqref="U130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -12387,8 +12387,8 @@
       <c r="S127" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="T127" s="6" t="s">
-        <v>183</v>
+      <c r="T127" s="64" t="s">
+        <v>2057</v>
       </c>
       <c r="U127" s="6"/>
       <c r="V127" s="37"/>

</xml_diff>

<commit_message>
nmv 11 01 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.2 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.2 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D273BB-2B40-4E1A-8C81-A6C41953E864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D3018B-F776-4F25-ACD3-99C89CC7034D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7032,9 +7032,9 @@
   <dimension ref="A1:X2500"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A222" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A375" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V233" sqref="V233"/>
+      <selection pane="bottomLeft" activeCell="U392" sqref="U392"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -21723,8 +21723,8 @@
       <c r="R391" s="6"/>
       <c r="S391" s="6"/>
       <c r="T391" s="6"/>
-      <c r="U391" s="6" t="s">
-        <v>122</v>
+      <c r="U391" s="64" t="s">
+        <v>173</v>
       </c>
       <c r="V391" s="37" t="s">
         <v>1411</v>

</xml_diff>

<commit_message>
nmv 13 01 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.2 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.2 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF33F691-447D-4FDC-B553-E89996883FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65945BB0-8141-4B5D-A0CF-8E22C953067E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7132" uniqueCount="2089">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7132" uniqueCount="2090">
   <si>
     <t>PS</t>
   </si>
@@ -6295,6 +6295,9 @@
   </si>
   <si>
     <t>aqkaqraqmitya#karam</t>
+  </si>
+  <si>
+    <t>maqrudBi#H</t>
   </si>
 </sst>
 </file>
@@ -7029,9 +7032,9 @@
   <dimension ref="A1:X2500"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A963" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1185" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N977" sqref="N977"/>
+      <selection pane="bottomLeft" activeCell="N1200" sqref="N1200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -49041,7 +49044,7 @@
         <v>315</v>
       </c>
       <c r="N1200" s="37" t="s">
-        <v>536</v>
+        <v>2089</v>
       </c>
       <c r="O1200" s="6" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
nmv 14 01 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.2 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.2 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65945BB0-8141-4B5D-A0CF-8E22C953067E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCE3657-0032-4AC7-8EFF-8136937D1C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7132" uniqueCount="2090">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7131" uniqueCount="2090">
   <si>
     <t>PS</t>
   </si>
@@ -6528,7 +6528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -6748,6 +6748,9 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7032,9 +7035,9 @@
   <dimension ref="A1:X2500"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1185" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1404" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1200" sqref="N1200"/>
+      <selection pane="bottomLeft" activeCell="N1415" sqref="N1415:N1416"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -56217,7 +56220,7 @@
         <f t="shared" si="68"/>
         <v>208</v>
       </c>
-      <c r="N1415" s="67" t="s">
+      <c r="N1415" s="76" t="s">
         <v>202</v>
       </c>
       <c r="O1415" s="5"/>
@@ -56226,9 +56229,7 @@
       <c r="R1415" s="6"/>
       <c r="S1415" s="6"/>
       <c r="T1415" s="6"/>
-      <c r="U1415" s="6" t="s">
-        <v>87</v>
-      </c>
+      <c r="U1415" s="6"/>
       <c r="V1415" s="37"/>
     </row>
     <row r="1416" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56251,7 +56252,7 @@
         <f t="shared" si="68"/>
         <v>209</v>
       </c>
-      <c r="N1416" s="67" t="s">
+      <c r="N1416" s="76" t="s">
         <v>948</v>
       </c>
       <c r="O1416" s="6" t="s">

</xml_diff>

<commit_message>
nmv 10 03 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.2 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.2 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F66BB43-C79F-4B75-93C2-89C74A0A13A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E701ECCB-F19B-4D6B-8EEB-29E7ED18F75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7032,9 +7032,9 @@
   <dimension ref="A1:X2500"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A878" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V888" sqref="V888"/>
+      <selection pane="bottomLeft" activeCell="N179" sqref="N179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -14242,8 +14242,8 @@
         <f t="shared" si="8"/>
         <v>178</v>
       </c>
-      <c r="N179" s="65" t="s">
-        <v>229</v>
+      <c r="N179" s="72" t="s">
+        <v>415</v>
       </c>
       <c r="O179" s="5"/>
       <c r="P179" s="6"/>

</xml_diff>